<commit_message>
modify 知识体系.md：补充类的内存结构部分 Signed-off-by: anshu.wang.work@gmail.com <anshu.wang.work@gmail.com>
</commit_message>
<xml_diff>
--- a/问题优化与总结/彩票站/各种内容各种规范.xlsx
+++ b/问题优化与总结/彩票站/各种内容各种规范.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="11385" tabRatio="914" activeTab="8"/>
+    <workbookView windowWidth="22943" windowHeight="9804" tabRatio="914" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="修订与审核" sheetId="8" r:id="rId1"/>
@@ -710,9 +710,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ \￥* #,##0.00_ ;_ \￥* \-#,##0.00_ ;_ \￥* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -752,6 +752,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -759,22 +766,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -788,25 +780,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -822,14 +797,45 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -843,11 +849,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -863,35 +892,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -970,31 +970,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,31 +1018,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,19 +1066,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1072,79 +1144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1166,17 +1166,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1205,6 +1194,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1228,17 +1247,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1251,168 +1266,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1566,8 +1566,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7100570" y="15049500"/>
-          <a:ext cx="2022475" cy="2453640"/>
+          <a:off x="7305040" y="14447520"/>
+          <a:ext cx="2080260" cy="2362200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1624,8 +1624,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7100570" y="11635740"/>
-          <a:ext cx="2015490" cy="342265"/>
+          <a:off x="7272020" y="11170920"/>
+          <a:ext cx="2048510" cy="334645"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1683,8 +1683,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="8182610" y="12131040"/>
-          <a:ext cx="914400" cy="641985"/>
+          <a:off x="8387080" y="11650980"/>
+          <a:ext cx="914400" cy="611505"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst/>
@@ -1742,8 +1742,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9337040" y="11079480"/>
-          <a:ext cx="914400" cy="634365"/>
+          <a:off x="9599295" y="10637520"/>
+          <a:ext cx="914400" cy="611505"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst/>
@@ -1903,8 +1903,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9337040" y="11833860"/>
-          <a:ext cx="914400" cy="634365"/>
+          <a:off x="9599295" y="11361420"/>
+          <a:ext cx="914400" cy="611505"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst/>
@@ -1965,8 +1965,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7390130" y="15575280"/>
-          <a:ext cx="1485900" cy="1447800"/>
+          <a:off x="7594600" y="14958060"/>
+          <a:ext cx="1485900" cy="1386840"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -2018,8 +2018,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7390130" y="16703040"/>
-          <a:ext cx="731520" cy="320040"/>
+          <a:off x="7594600" y="16040100"/>
+          <a:ext cx="731520" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2077,8 +2077,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8134350" y="16708120"/>
-          <a:ext cx="731520" cy="320040"/>
+          <a:off x="8338820" y="16045180"/>
+          <a:ext cx="731520" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2235,8 +2235,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="3600000">
-          <a:off x="8138795" y="18938240"/>
-          <a:ext cx="210185" cy="121920"/>
+          <a:off x="8347075" y="18180050"/>
+          <a:ext cx="202565" cy="121920"/>
         </a:xfrm>
         <a:prstGeom prst="curvedDownArrow">
           <a:avLst/>
@@ -2292,8 +2292,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9276080" y="18552795"/>
-          <a:ext cx="1432560" cy="441960"/>
+          <a:off x="9538335" y="17813655"/>
+          <a:ext cx="1432560" cy="426720"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst/>
@@ -2453,8 +2453,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7778750" y="12857480"/>
-          <a:ext cx="713740" cy="514350"/>
+          <a:off x="7983220" y="12346940"/>
+          <a:ext cx="713740" cy="491490"/>
           <a:chOff x="12228" y="20233"/>
           <a:chExt cx="1124" cy="810"/>
         </a:xfrm>
@@ -2667,8 +2667,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9340215" y="12751435"/>
-          <a:ext cx="914400" cy="634365"/>
+          <a:off x="9602470" y="12248515"/>
+          <a:ext cx="914400" cy="603885"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout1">
           <a:avLst>
@@ -3080,16 +3080,16 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="9.38095238095238" customWidth="1"/>
-    <col min="2" max="2" width="8.88571428571429" customWidth="1"/>
+    <col min="1" max="1" width="9.37962962962963" customWidth="1"/>
+    <col min="2" max="2" width="8.88888888888889" customWidth="1"/>
     <col min="3" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="8.88571428571429" customWidth="1"/>
-    <col min="8" max="8" width="10.3714285714286" customWidth="1"/>
-    <col min="9" max="9" width="8.87619047619048" customWidth="1"/>
+    <col min="5" max="5" width="8.88888888888889" customWidth="1"/>
+    <col min="8" max="8" width="10.3703703703704" customWidth="1"/>
+    <col min="9" max="9" width="8.87962962962963" customWidth="1"/>
     <col min="10" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="8.87619047619048" customWidth="1"/>
+    <col min="12" max="12" width="8.87962962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="7:12">
@@ -3148,7 +3148,7 @@
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -3164,12 +3164,12 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8952380952381" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="9.66666666666667" customWidth="1"/>
-    <col min="5" max="5" width="13.1047619047619" customWidth="1"/>
-    <col min="6" max="6" width="12.5619047619048" customWidth="1"/>
-    <col min="7" max="7" width="11.8952380952381" customWidth="1"/>
+    <col min="5" max="5" width="13.1018518518519" customWidth="1"/>
+    <col min="6" max="6" width="12.5648148148148" customWidth="1"/>
+    <col min="7" max="7" width="11.8981481481481" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:4">
@@ -3553,11 +3553,11 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="15.752380952381" customWidth="1"/>
-    <col min="5" max="5" width="14.8857142857143" customWidth="1"/>
-    <col min="6" max="6" width="17.1333333333333" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="14.8888888888889" customWidth="1"/>
+    <col min="6" max="6" width="17.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:13">
@@ -4195,10 +4195,10 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8952380952381" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="4" max="4" width="14.1047619047619" customWidth="1"/>
-    <col min="5" max="5" width="17.5619047619048" customWidth="1"/>
+    <col min="4" max="4" width="14.1018518518519" customWidth="1"/>
+    <col min="5" max="5" width="17.5648148148148" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:3">
@@ -4273,13 +4273,13 @@
       <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8952380952381" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="6" width="18.6666666666667" customWidth="1"/>
-    <col min="8" max="9" width="17.2285714285714" customWidth="1"/>
-    <col min="10" max="10" width="30.2285714285714" customWidth="1"/>
-    <col min="11" max="11" width="33.1047619047619" customWidth="1"/>
-    <col min="14" max="14" width="10.4285714285714" customWidth="1"/>
+    <col min="8" max="9" width="17.2314814814815" customWidth="1"/>
+    <col min="10" max="10" width="30.2314814814815" customWidth="1"/>
+    <col min="11" max="11" width="33.1018518518519" customWidth="1"/>
+    <col min="14" max="14" width="10.4259259259259" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="6:6">
@@ -4841,13 +4841,13 @@
   <sheetPr/>
   <dimension ref="G8:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8952380952381" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="7" max="7" width="22.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="22.1388888888889" customWidth="1"/>
     <col min="8" max="8" width="9"/>
   </cols>
   <sheetData>
@@ -5039,9 +5039,9 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="6" max="6" width="20.8952380952381" customWidth="1"/>
+    <col min="6" max="6" width="20.8981481481481" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="6:6">
@@ -5070,14 +5070,14 @@
   <sheetPr/>
   <dimension ref="C2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="4" max="4" width="17.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="12.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="17.4259259259259" customWidth="1"/>
+    <col min="5" max="5" width="12.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:4">

</xml_diff>